<commit_message>
add banco.csv and update banco.xlsx
</commit_message>
<xml_diff>
--- a/banco.xlsx
+++ b/banco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRYAN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inversion\Generador de Examenes IA\bank\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1339,17 +1339,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1657,14 +1651,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81:H81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
@@ -1681,7 +1675,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1715,14 +1709,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
@@ -1757,7 +1751,7 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D3" t="s">
@@ -1785,14 +1779,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>98</v>
       </c>
       <c r="D4" t="s">
@@ -1820,14 +1814,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
@@ -1862,7 +1856,7 @@
       <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
@@ -1897,7 +1891,7 @@
       <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D7" t="s">
@@ -1925,14 +1919,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>89</v>
       </c>
       <c r="D8" t="s">
@@ -1967,7 +1961,7 @@
       <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>90</v>
       </c>
       <c r="D9" t="s">
@@ -2002,7 +1996,7 @@
       <c r="B10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D10" t="s">
@@ -2037,7 +2031,7 @@
       <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D11" t="s">
@@ -2072,7 +2066,7 @@
       <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D12" t="s">
@@ -2107,7 +2101,7 @@
       <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>93</v>
       </c>
       <c r="D13" t="s">
@@ -2135,14 +2129,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>94</v>
       </c>
       <c r="D14" t="s">
@@ -2170,14 +2164,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D15" t="s">
@@ -2212,7 +2206,7 @@
       <c r="B16" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D16" t="s">
@@ -2240,14 +2234,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D17" t="s">
@@ -2275,14 +2269,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D18" t="s">
@@ -2310,14 +2304,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D19" t="s">
@@ -2345,14 +2339,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>128</v>
       </c>
       <c r="D20" t="s">
@@ -2380,14 +2374,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D21" t="s">
@@ -2422,7 +2416,7 @@
       <c r="B22" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D22">
@@ -2449,7 +2443,7 @@
       <c r="K22" t="s">
         <v>135</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="1" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2460,7 +2454,7 @@
       <c r="B23" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>139</v>
       </c>
       <c r="D23" t="s">
@@ -2487,7 +2481,7 @@
       <c r="K23" t="s">
         <v>135</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="1" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2498,7 +2492,7 @@
       <c r="B24" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D24">
@@ -2533,7 +2527,7 @@
       <c r="B25" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D25">
@@ -2560,7 +2554,7 @@
       <c r="K25" t="s">
         <v>135</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="1" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2571,7 +2565,7 @@
       <c r="B26" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D26">
@@ -2598,7 +2592,7 @@
       <c r="K26" t="s">
         <v>135</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="1" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2609,7 +2603,7 @@
       <c r="B27" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="3" t="s">
         <v>151</v>
       </c>
       <c r="D27">
@@ -2636,18 +2630,18 @@
       <c r="K27" t="s">
         <v>135</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>153</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D28">
@@ -2675,14 +2669,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>153</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D29">
@@ -2710,14 +2704,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>153</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="3" t="s">
         <v>162</v>
       </c>
       <c r="D30">
@@ -2752,7 +2746,7 @@
       <c r="B31" t="s">
         <v>153</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D31" t="s">
@@ -2780,14 +2774,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>164</v>
       </c>
       <c r="D32">
@@ -2822,7 +2816,7 @@
       <c r="B33" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="3" t="s">
         <v>165</v>
       </c>
       <c r="D33">
@@ -2849,18 +2843,18 @@
       <c r="K33" t="s">
         <v>135</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="L33" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>163</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D34">
@@ -2895,7 +2889,7 @@
       <c r="B35" t="s">
         <v>163</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="3" t="s">
         <v>168</v>
       </c>
       <c r="D35" t="s">
@@ -2913,7 +2907,7 @@
       <c r="H35" t="s">
         <v>173</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="2" t="s">
         <v>170</v>
       </c>
       <c r="J35" t="s">
@@ -2922,7 +2916,7 @@
       <c r="K35" t="s">
         <v>135</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="L35" s="1" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2933,7 +2927,7 @@
       <c r="B36" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="3" t="s">
         <v>176</v>
       </c>
       <c r="D36">
@@ -2968,7 +2962,7 @@
       <c r="B37" t="s">
         <v>175</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="3" t="s">
         <v>177</v>
       </c>
       <c r="D37">
@@ -3003,7 +2997,7 @@
       <c r="B38" t="s">
         <v>178</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>179</v>
       </c>
       <c r="D38">
@@ -3030,18 +3024,18 @@
       <c r="K38" t="s">
         <v>135</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="L38" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>178</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D39">
@@ -3068,18 +3062,18 @@
       <c r="K39" t="s">
         <v>135</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>178</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="3" t="s">
         <v>188</v>
       </c>
       <c r="D40" t="s">
@@ -3107,14 +3101,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>178</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="3" t="s">
         <v>189</v>
       </c>
       <c r="D41">
@@ -3142,14 +3136,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>190</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D42" t="s">
@@ -3177,14 +3171,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>190</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="3" t="s">
         <v>201</v>
       </c>
       <c r="D43" t="s">
@@ -3212,7 +3206,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3247,14 +3241,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>190</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="3" t="s">
         <v>214</v>
       </c>
       <c r="D45" t="s">
@@ -3282,14 +3276,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>190</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="3" t="s">
         <v>220</v>
       </c>
       <c r="D46" t="s">
@@ -3317,14 +3311,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="3" t="s">
         <v>226</v>
       </c>
       <c r="D47" t="s">
@@ -3352,14 +3346,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>227</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="3" t="s">
         <v>228</v>
       </c>
       <c r="D48">
@@ -3387,14 +3381,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>227</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="3" t="s">
         <v>229</v>
       </c>
       <c r="D49">
@@ -3422,14 +3416,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>227</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D50">
@@ -3457,14 +3451,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>227</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="3" t="s">
         <v>231</v>
       </c>
       <c r="D51">
@@ -3492,14 +3486,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>227</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="3" t="s">
         <v>232</v>
       </c>
       <c r="D52" t="s">
@@ -3534,7 +3528,7 @@
       <c r="B53" t="s">
         <v>227</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="3" t="s">
         <v>238</v>
       </c>
       <c r="D53" t="s">
@@ -3569,7 +3563,7 @@
       <c r="B54" t="s">
         <v>244</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="3" t="s">
         <v>251</v>
       </c>
       <c r="D54" t="s">
@@ -3596,11 +3590,11 @@
       <c r="K54" t="s">
         <v>135</v>
       </c>
-      <c r="L54" s="2" t="s">
+      <c r="L54" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3634,7 +3628,7 @@
       <c r="K55" t="s">
         <v>135</v>
       </c>
-      <c r="L55" s="2" t="s">
+      <c r="L55" s="1" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3645,7 +3639,7 @@
       <c r="B56" t="s">
         <v>244</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="3" t="s">
         <v>259</v>
       </c>
       <c r="D56" t="s">
@@ -3673,14 +3667,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>244</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="3" t="s">
         <v>270</v>
       </c>
       <c r="D57" t="s">
@@ -3707,7 +3701,7 @@
       <c r="K57" t="s">
         <v>135</v>
       </c>
-      <c r="L57" s="2" t="s">
+      <c r="L57" s="1" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3718,7 +3712,7 @@
       <c r="B58" t="s">
         <v>271</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="3" t="s">
         <v>272</v>
       </c>
       <c r="D58" t="s">
@@ -3753,7 +3747,7 @@
       <c r="B59" t="s">
         <v>271</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="3" t="s">
         <v>278</v>
       </c>
       <c r="D59" t="s">
@@ -3788,7 +3782,7 @@
       <c r="B60" t="s">
         <v>271</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="3" t="s">
         <v>284</v>
       </c>
       <c r="D60" t="s">
@@ -3816,14 +3810,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>271</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="3" t="s">
         <v>290</v>
       </c>
       <c r="D61" t="s">
@@ -3858,7 +3852,7 @@
       <c r="B62" t="s">
         <v>296</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="3" t="s">
         <v>297</v>
       </c>
       <c r="D62" t="s">
@@ -3893,7 +3887,7 @@
       <c r="B63" t="s">
         <v>296</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="3" t="s">
         <v>304</v>
       </c>
       <c r="D63" t="s">
@@ -3928,7 +3922,7 @@
       <c r="B64" t="s">
         <v>310</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="3" t="s">
         <v>311</v>
       </c>
       <c r="D64" t="s">
@@ -3956,14 +3950,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>310</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="3" t="s">
         <v>317</v>
       </c>
       <c r="D65" t="s">
@@ -3998,7 +3992,7 @@
       <c r="B66" t="s">
         <v>323</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="3" t="s">
         <v>324</v>
       </c>
       <c r="D66" t="s">
@@ -4033,7 +4027,7 @@
       <c r="B67" t="s">
         <v>323</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="3" t="s">
         <v>330</v>
       </c>
       <c r="D67" t="s">
@@ -4068,7 +4062,7 @@
       <c r="B68" t="s">
         <v>323</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="3" t="s">
         <v>336</v>
       </c>
       <c r="D68" t="s">
@@ -4103,7 +4097,7 @@
       <c r="B69" t="s">
         <v>323</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="3" t="s">
         <v>342</v>
       </c>
       <c r="D69" t="s">
@@ -4138,7 +4132,7 @@
       <c r="B70" t="s">
         <v>348</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="3" t="s">
         <v>349</v>
       </c>
       <c r="D70" t="s">
@@ -4166,14 +4160,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>348</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="3" t="s">
         <v>355</v>
       </c>
       <c r="D71" t="s">
@@ -4208,7 +4202,7 @@
       <c r="B72" t="s">
         <v>348</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="3" t="s">
         <v>361</v>
       </c>
       <c r="D72" t="s">
@@ -4243,7 +4237,7 @@
       <c r="B73" t="s">
         <v>190</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="3" t="s">
         <v>367</v>
       </c>
       <c r="D73" t="s">
@@ -4278,7 +4272,7 @@
       <c r="B74" t="s">
         <v>373</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="3" t="s">
         <v>374</v>
       </c>
       <c r="D74" t="s">
@@ -4306,14 +4300,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>373</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="3" t="s">
         <v>380</v>
       </c>
       <c r="D75" t="s">
@@ -4348,7 +4342,7 @@
       <c r="B76" t="s">
         <v>386</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="3" t="s">
         <v>387</v>
       </c>
       <c r="D76" t="s">
@@ -4383,7 +4377,7 @@
       <c r="B77" t="s">
         <v>386</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="3" t="s">
         <v>393</v>
       </c>
       <c r="D77" t="s">
@@ -4411,14 +4405,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>399</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="3" t="s">
         <v>400</v>
       </c>
       <c r="D78" t="s">
@@ -4453,7 +4447,7 @@
       <c r="B79" t="s">
         <v>399</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="3" t="s">
         <v>406</v>
       </c>
       <c r="D79" t="s">
@@ -4488,7 +4482,7 @@
       <c r="B80" t="s">
         <v>399</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="3" t="s">
         <v>412</v>
       </c>
       <c r="D80" t="s">
@@ -4516,14 +4510,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>399</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="3" t="s">
         <v>418</v>
       </c>
       <c r="D81" t="s">

</xml_diff>